<commit_message>
restructured directories & added placeholders
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Notes</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>**Quadrant Photodiode</t>
+  </si>
+  <si>
+    <t>http://www.mikroe.com/click/camera/</t>
+  </si>
+  <si>
+    <t>MIKROE-1816</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/MikroElektronika/MIKROE-1816/?qs=m96fseALk3XQncba6Dp5Ww%3D%3D</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/mikroelektronika/MIKROE-1816/1471-1406-ND/5233456</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1180,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1303,7 +1315,9 @@
       <c r="D4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" s="14" t="s">
         <v>9</v>
       </c>
@@ -1313,9 +1327,15 @@
       <c r="H4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
+      <c r="I4" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12"/>
@@ -1457,11 +1477,14 @@
     <hyperlink ref="K2" r:id="rId6"/>
     <hyperlink ref="J8" r:id="rId7"/>
     <hyperlink ref="I8" r:id="rId8"/>
+    <hyperlink ref="I4" r:id="rId9"/>
+    <hyperlink ref="J4" r:id="rId10"/>
+    <hyperlink ref="K4" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more datasheets and dvt items and rework #1 for potentiometer fix
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -1035,9 +1035,6 @@
     <t>2.2nF</t>
   </si>
   <si>
-    <t>2pF</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -1090,6 +1087,9 @@
   </si>
   <si>
     <t>DS1, DS2, DS4, DS8</t>
+  </si>
+  <si>
+    <t>2.2pF</t>
   </si>
 </sst>
 </file>
@@ -2614,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2757,7 +2757,7 @@
         <v>153</v>
       </c>
       <c r="I4" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="J4" s="44" t="s">
         <v>303</v>
@@ -2790,7 +2790,7 @@
         <v>153</v>
       </c>
       <c r="I5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J5" s="44" t="s">
         <v>306</v>
@@ -2823,7 +2823,7 @@
         <v>153</v>
       </c>
       <c r="I6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J6" s="44" t="s">
         <v>308</v>
@@ -2856,7 +2856,7 @@
         <v>153</v>
       </c>
       <c r="I7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J7" s="44" t="s">
         <v>332</v>
@@ -3066,7 +3066,7 @@
         <v>183</v>
       </c>
       <c r="G14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H14" t="s">
         <v>154</v>
@@ -3327,7 +3327,7 @@
         <v>153</v>
       </c>
       <c r="I22" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J22" s="44" t="s">
         <v>313</v>
@@ -3360,7 +3360,7 @@
         <v>153</v>
       </c>
       <c r="I23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J23" s="44" t="s">
         <v>312</v>
@@ -3393,7 +3393,7 @@
         <v>153</v>
       </c>
       <c r="I24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J24" s="44" t="s">
         <v>314</v>
@@ -3426,7 +3426,7 @@
         <v>153</v>
       </c>
       <c r="I25" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J25" s="44" t="s">
         <v>317</v>
@@ -3459,7 +3459,7 @@
         <v>153</v>
       </c>
       <c r="I26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J26" s="44" t="s">
         <v>318</v>
@@ -3492,7 +3492,7 @@
         <v>153</v>
       </c>
       <c r="I27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J27" s="44" t="s">
         <v>319</v>
@@ -3525,7 +3525,7 @@
         <v>153</v>
       </c>
       <c r="I28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J28" s="44" t="s">
         <v>320</v>
@@ -3558,7 +3558,7 @@
         <v>153</v>
       </c>
       <c r="I29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J29" s="44" t="s">
         <v>325</v>
@@ -3591,7 +3591,7 @@
         <v>153</v>
       </c>
       <c r="I30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="J30" s="44" t="s">
         <v>327</v>
@@ -3624,7 +3624,7 @@
         <v>159</v>
       </c>
       <c r="I31" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J31" s="44" t="s">
         <v>329</v>
@@ -3657,7 +3657,7 @@
         <v>154</v>
       </c>
       <c r="I32" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J32" s="44" t="s">
         <v>331</v>
@@ -3805,7 +3805,7 @@
         <v>104</v>
       </c>
       <c r="F38" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G38" t="s">
         <v>36</v>
@@ -3814,7 +3814,7 @@
         <v>119</v>
       </c>
       <c r="I38" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J38" s="44" t="s">
         <v>102</v>
@@ -3878,7 +3878,7 @@
         <v>116</v>
       </c>
       <c r="J40" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
@@ -3921,7 +3921,7 @@
         <v>0.6</v>
       </c>
       <c r="E42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F42">
         <v>7682</v>
@@ -3947,7 +3947,7 @@
         <v>0.26</v>
       </c>
       <c r="E43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F43">
         <v>4688</v>
@@ -4047,8 +4047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
debugged servo current surge issue and created workaround plan
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\MS\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\Thesis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="369">
   <si>
     <t>MFR</t>
   </si>
@@ -1090,6 +1090,51 @@
   </si>
   <si>
     <t>2.2pF</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/panasonic-bsg/CR1632/P036-ND/269743</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>CR1632</t>
+  </si>
+  <si>
+    <t>External Battery</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>16mm diameter x 2.2mm</t>
+  </si>
+  <si>
+    <t>4700uF</t>
+  </si>
+  <si>
+    <t>EEU-FC1A472L</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/panasonic-electronic-components/EEU-FC1A472L/P10236-ND/266246</t>
+  </si>
+  <si>
+    <t>C/20%/10V</t>
+  </si>
+  <si>
+    <t>Heat Shrink for External Battery</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>25.4mm diameter</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/3m/FP-301-1--BL-100-/FP100K-5-ND/116997</t>
+  </si>
+  <si>
+    <t>FP-301 1" BL 100'</t>
   </si>
 </sst>
 </file>
@@ -2612,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2708,7 +2753,7 @@
         <v>0.18</v>
       </c>
       <c r="D3" s="45">
-        <f t="shared" ref="D3:D32" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D33" si="0">B3*C3</f>
         <v>0.36</v>
       </c>
       <c r="E3" t="s">
@@ -2864,473 +2909,467 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>203</v>
+        <v>363</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" s="45">
-        <v>0.15</v>
+        <v>1.43</v>
       </c>
       <c r="D8" s="45">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>5.72</v>
       </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>355</v>
       </c>
       <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>285</v>
-      </c>
-      <c r="H8" t="s">
-        <v>93</v>
+        <v>361</v>
+      </c>
+      <c r="I8" t="s">
+        <v>360</v>
       </c>
       <c r="J8" s="44" t="s">
-        <v>284</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" s="45">
-        <v>0.83</v>
+        <v>0.15</v>
       </c>
       <c r="D9" s="45">
         <f t="shared" si="0"/>
-        <v>3.32</v>
+        <v>0.6</v>
       </c>
       <c r="E9" t="s">
         <v>87</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="G9" t="s">
-        <v>233</v>
+        <v>285</v>
       </c>
       <c r="H9" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="J9" s="44" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>142</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C10" s="45">
-        <v>3.19</v>
+        <v>0.83</v>
       </c>
       <c r="D10" s="45">
         <f t="shared" si="0"/>
-        <v>6.38</v>
+        <v>3.32</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>214</v>
+        <v>123</v>
       </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="H10" t="s">
-        <v>215</v>
-      </c>
-      <c r="I10" t="s">
-        <v>279</v>
+        <v>123</v>
       </c>
       <c r="J10" s="44" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11" s="45">
-        <v>0.34</v>
+        <v>3.19</v>
       </c>
       <c r="D11" s="45">
         <f t="shared" si="0"/>
-        <v>1.36</v>
+        <v>6.38</v>
       </c>
       <c r="E11" t="s">
-        <v>266</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="G11" t="s">
-        <v>286</v>
+        <v>216</v>
       </c>
       <c r="H11" t="s">
-        <v>154</v>
+        <v>215</v>
+      </c>
+      <c r="I11" t="s">
+        <v>279</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>265</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" s="45">
-        <v>0.21</v>
+        <v>0.34</v>
       </c>
       <c r="D12" s="45">
         <f t="shared" si="0"/>
-        <v>0.42</v>
+        <v>1.36</v>
       </c>
       <c r="E12" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
       <c r="F12" t="s">
-        <v>236</v>
+        <v>175</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>286</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="J12" s="44" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>267</v>
+        <v>234</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="45">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="D13" s="45">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.42</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="F13" t="s">
-        <v>178</v>
+        <v>236</v>
       </c>
       <c r="G13" t="s">
-        <v>287</v>
+        <v>144</v>
       </c>
       <c r="H13" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="J13" s="44" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C14" s="45">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="D14" s="45">
         <f t="shared" si="0"/>
-        <v>1.36</v>
+        <v>0.72</v>
       </c>
       <c r="E14" t="s">
         <v>266</v>
       </c>
       <c r="F14" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G14" t="s">
-        <v>352</v>
+        <v>287</v>
       </c>
       <c r="H14" t="s">
         <v>154</v>
       </c>
       <c r="J14" s="44" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>211</v>
+        <v>268</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15" s="45">
-        <v>5.95</v>
+        <v>0.17</v>
       </c>
       <c r="D15" s="45">
         <f t="shared" si="0"/>
-        <v>11.9</v>
+        <v>1.36</v>
       </c>
       <c r="E15" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
       <c r="G15" t="s">
-        <v>212</v>
+        <v>352</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="J15" s="44" t="s">
-        <v>111</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>274</v>
+        <v>211</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" s="45">
-        <v>2.1</v>
+        <v>5.95</v>
       </c>
       <c r="D16" s="45">
         <f t="shared" si="0"/>
-        <v>8.4</v>
+        <v>11.9</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>213</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="G16" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="H16" t="s">
-        <v>190</v>
+        <v>113</v>
       </c>
       <c r="J16" s="44" t="s">
-        <v>293</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>237</v>
+        <v>274</v>
       </c>
       <c r="B17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" s="45">
-        <v>0.52</v>
+        <v>2.1</v>
       </c>
       <c r="D17" s="45">
         <f t="shared" si="0"/>
-        <v>1.04</v>
+        <v>8.4</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="F17" t="s">
-        <v>209</v>
+        <v>90</v>
       </c>
       <c r="G17" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="H17" t="s">
-        <v>207</v>
-      </c>
-      <c r="I17" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="J17" s="44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" s="45">
-        <v>0.42</v>
+        <v>0.52</v>
       </c>
       <c r="D18" s="45">
         <f t="shared" si="0"/>
-        <v>0.84</v>
+        <v>1.04</v>
       </c>
       <c r="E18" t="s">
         <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H18" t="s">
         <v>207</v>
       </c>
       <c r="I18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J18" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>239</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" s="45">
-        <v>6.21</v>
+        <v>0.42</v>
       </c>
       <c r="D19" s="45">
         <f t="shared" si="0"/>
-        <v>24.84</v>
+        <v>0.84</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
       <c r="G19" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="I19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J19" s="44" t="s">
-        <v>59</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>48</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C20" s="45">
-        <v>31.42</v>
+        <v>6.21</v>
       </c>
       <c r="D20" s="45">
         <f t="shared" si="0"/>
-        <v>62.84</v>
+        <v>24.84</v>
       </c>
       <c r="E20" t="s">
-        <v>200</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>243</v>
       </c>
       <c r="G20" t="s">
-        <v>199</v>
+        <v>241</v>
       </c>
       <c r="H20" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="I20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J20" s="44" t="s">
-        <v>296</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" s="45">
-        <v>52.25</v>
+        <v>31.42</v>
       </c>
       <c r="D21" s="45">
         <f t="shared" si="0"/>
-        <v>104.5</v>
+        <v>62.84</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>197</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H21" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I21" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="J21" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>249</v>
+        <v>34</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="45">
-        <v>0.1</v>
+        <v>52.25</v>
       </c>
       <c r="D22" s="45">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>104.5</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>311</v>
+        <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>250</v>
+        <v>202</v>
       </c>
       <c r="H22" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="I22" t="s">
-        <v>338</v>
+        <v>276</v>
       </c>
       <c r="J22" s="44" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.4">
@@ -3338,32 +3377,32 @@
         <v>249</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C23" s="45">
         <v>0.1</v>
       </c>
       <c r="D23" s="45">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E23" t="s">
         <v>73</v>
       </c>
       <c r="F23" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G23" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="H23" t="s">
         <v>153</v>
       </c>
       <c r="I23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J23" s="44" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
@@ -3371,32 +3410,32 @@
         <v>249</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C24" s="45">
         <v>0.1</v>
       </c>
       <c r="D24" s="45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E24" t="s">
         <v>73</v>
       </c>
       <c r="F24" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G24" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H24" t="s">
         <v>153</v>
       </c>
       <c r="I24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J24" s="44" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
@@ -3404,32 +3443,32 @@
         <v>249</v>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C25" s="45">
         <v>0.1</v>
       </c>
       <c r="D25" s="45">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>73</v>
       </c>
       <c r="F25" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="G25" t="s">
-        <v>161</v>
+        <v>257</v>
       </c>
       <c r="H25" t="s">
         <v>153</v>
       </c>
       <c r="I25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J25" s="44" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.4">
@@ -3437,32 +3476,32 @@
         <v>249</v>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C26" s="45">
         <v>0.1</v>
       </c>
       <c r="D26" s="45">
         <f t="shared" si="0"/>
-        <v>0.60000000000000009</v>
+        <v>0.2</v>
       </c>
       <c r="E26" t="s">
         <v>73</v>
       </c>
       <c r="F26" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G26" t="s">
-        <v>260</v>
+        <v>161</v>
       </c>
       <c r="H26" t="s">
         <v>153</v>
       </c>
       <c r="I26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="J26" s="44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.4">
@@ -3470,32 +3509,32 @@
         <v>249</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C27" s="45">
         <v>0.1</v>
       </c>
       <c r="D27" s="45">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="E27" t="s">
         <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G27" t="s">
-        <v>167</v>
+        <v>260</v>
       </c>
       <c r="H27" t="s">
         <v>153</v>
       </c>
       <c r="I27" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="J27" s="44" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
@@ -3516,19 +3555,19 @@
         <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="G28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H28" t="s">
         <v>153</v>
       </c>
       <c r="I28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J28" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
@@ -3536,32 +3575,32 @@
         <v>249</v>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C29" s="45">
         <v>0.1</v>
       </c>
       <c r="D29" s="45">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E29" t="s">
         <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="G29" t="s">
-        <v>263</v>
+        <v>170</v>
       </c>
       <c r="H29" t="s">
         <v>153</v>
       </c>
       <c r="I29" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="J29" s="44" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.4">
@@ -3582,198 +3621,199 @@
         <v>73</v>
       </c>
       <c r="F30" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H30" t="s">
         <v>153</v>
       </c>
       <c r="I30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J30" s="44" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C31" s="45">
-        <v>1.17</v>
+        <v>0.1</v>
       </c>
       <c r="D31" s="45">
         <f t="shared" si="0"/>
-        <v>2.34</v>
+        <v>0.4</v>
       </c>
       <c r="E31" t="s">
         <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>83</v>
+        <v>328</v>
       </c>
       <c r="G31" t="s">
-        <v>160</v>
+        <v>264</v>
       </c>
       <c r="H31" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="I31" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="J31" s="44" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" s="45">
-        <v>0.79</v>
+        <v>1.17</v>
       </c>
       <c r="D32" s="45">
         <f t="shared" si="0"/>
-        <v>1.58</v>
+        <v>2.34</v>
       </c>
       <c r="E32" t="s">
         <v>73</v>
       </c>
       <c r="F32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+      <c r="H32" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" t="s">
+        <v>340</v>
+      </c>
+      <c r="J32" s="44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>253</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="45">
+        <v>0.79</v>
+      </c>
+      <c r="D33" s="45">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" t="s">
         <v>330</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G33" t="s">
         <v>155</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H33" t="s">
         <v>154</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I33" t="s">
         <v>347</v>
       </c>
-      <c r="J32" s="44" t="s">
+      <c r="J33" s="44" t="s">
         <v>331</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>232</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="46">
-        <v>19.149999999999999</v>
-      </c>
-      <c r="D34" s="46">
-        <v>19.149999999999999</v>
-      </c>
-      <c r="E34" t="s">
-        <v>118</v>
-      </c>
-      <c r="F34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" t="s">
-        <v>129</v>
-      </c>
-      <c r="J34" s="44" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>232</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" s="46">
-        <v>39</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="D35" s="46">
-        <v>78</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="E35" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="F35" t="s">
-        <v>26</v>
+        <v>127</v>
       </c>
       <c r="G35" t="s">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="H35" t="s">
-        <v>120</v>
-      </c>
-      <c r="I35" t="s">
-        <v>12</v>
+        <v>129</v>
       </c>
       <c r="J35" s="44" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>231</v>
+        <v>9</v>
       </c>
       <c r="B36">
         <v>2</v>
       </c>
       <c r="C36" s="46">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D36" s="46">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G36" t="s">
         <v>8</v>
       </c>
       <c r="H36" t="s">
-        <v>19</v>
+        <v>120</v>
       </c>
       <c r="I36" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J36" s="44" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" s="46">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D37" s="46">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
         <v>20</v>
       </c>
       <c r="F37" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -3782,264 +3822,358 @@
         <v>19</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J37" s="44" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>230</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" s="46">
-        <v>19.989999999999998</v>
+        <v>39</v>
       </c>
       <c r="D38" s="46">
-        <v>19.989999999999998</v>
+        <v>78</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="F38" t="s">
-        <v>348</v>
+        <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="I38" t="s">
-        <v>349</v>
+        <v>17</v>
       </c>
       <c r="J38" s="44" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>282</v>
+        <v>101</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" s="46">
-        <v>29.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D39" s="46">
-        <v>59.98</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="E39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>348</v>
       </c>
       <c r="G39" t="s">
         <v>36</v>
       </c>
       <c r="H39" t="s">
-        <v>133</v>
+        <v>119</v>
+      </c>
+      <c r="I39" t="s">
+        <v>349</v>
       </c>
       <c r="J39" s="44" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>229</v>
+        <v>282</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
       <c r="C40" s="46">
-        <v>6.49</v>
+        <v>29.99</v>
       </c>
       <c r="D40" s="46">
-        <v>19.3</v>
+        <v>59.98</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="G40" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H40" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="J40" s="44" t="s">
-        <v>350</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" s="46">
-        <v>0.41</v>
+        <v>6.49</v>
       </c>
       <c r="D41" s="46">
-        <v>0.82</v>
+        <v>19.3</v>
       </c>
       <c r="E41" t="s">
-        <v>220</v>
+        <v>118</v>
       </c>
       <c r="F41" t="s">
-        <v>224</v>
+        <v>118</v>
       </c>
       <c r="G41" t="s">
-        <v>219</v>
+        <v>50</v>
+      </c>
+      <c r="H41" t="s">
+        <v>117</v>
+      </c>
+      <c r="I41" t="s">
+        <v>116</v>
       </c>
       <c r="J41" s="44" t="s">
-        <v>221</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C42" s="46">
-        <v>0.15</v>
+        <v>0.41</v>
       </c>
       <c r="D42" s="46">
-        <v>0.6</v>
+        <v>0.82</v>
       </c>
       <c r="E42" t="s">
-        <v>351</v>
-      </c>
-      <c r="F42">
-        <v>7682</v>
+        <v>220</v>
+      </c>
+      <c r="F42" t="s">
+        <v>224</v>
       </c>
       <c r="G42" t="s">
         <v>219</v>
       </c>
       <c r="J42" s="44" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C43" s="46">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="D43" s="46">
-        <v>0.26</v>
+        <v>0.6</v>
       </c>
       <c r="E43" t="s">
         <v>351</v>
       </c>
       <c r="F43">
-        <v>4688</v>
+        <v>7682</v>
       </c>
       <c r="G43" t="s">
         <v>219</v>
       </c>
       <c r="J43" s="44" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
+        <v>227</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" s="46">
+        <v>0.13</v>
+      </c>
+      <c r="D44" s="46">
+        <v>0.26</v>
+      </c>
+      <c r="E44" t="s">
+        <v>351</v>
+      </c>
+      <c r="F44">
+        <v>4688</v>
+      </c>
+      <c r="G44" t="s">
+        <v>219</v>
+      </c>
+      <c r="J44" s="44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>228</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>3</v>
       </c>
-      <c r="C44" s="46">
+      <c r="C45" s="46">
         <v>3.95</v>
       </c>
-      <c r="D44" s="46">
+      <c r="D45" s="46">
         <v>11.850000000000001</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E45" t="s">
         <v>139</v>
       </c>
-      <c r="F44">
+      <c r="F45">
         <v>1949</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G45" t="s">
         <v>88</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>138</v>
       </c>
-      <c r="J44" s="44" t="s">
+      <c r="J45" s="44" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D45" s="6">
-        <f>SUM(D2:D44)</f>
-        <v>575.41000000000008</v>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>357</v>
+      </c>
+      <c r="B46">
+        <v>8</v>
+      </c>
+      <c r="C46" s="45">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D46" s="45">
+        <f>B46*C46</f>
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="E46" t="s">
+        <v>355</v>
+      </c>
+      <c r="F46" t="s">
+        <v>356</v>
+      </c>
+      <c r="G46" t="s">
+        <v>358</v>
+      </c>
+      <c r="H46" t="s">
+        <v>359</v>
+      </c>
+      <c r="J46" s="44" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>364</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" s="45">
+        <v>5.91</v>
+      </c>
+      <c r="D47" s="45">
+        <f>B47*C47</f>
+        <v>5.91</v>
+      </c>
+      <c r="E47" t="s">
+        <v>365</v>
+      </c>
+      <c r="F47" t="s">
+        <v>368</v>
+      </c>
+      <c r="G47" t="s">
+        <v>358</v>
+      </c>
+      <c r="H47" t="s">
+        <v>366</v>
+      </c>
+      <c r="J47" s="44" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D48" s="6">
+        <f>SUM(D2:D47)</f>
+        <v>595.76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1"/>
-    <hyperlink ref="J8" r:id="rId2"/>
-    <hyperlink ref="J9" r:id="rId3"/>
-    <hyperlink ref="J11" r:id="rId4"/>
-    <hyperlink ref="J25" r:id="rId5"/>
-    <hyperlink ref="J29" r:id="rId6"/>
-    <hyperlink ref="J30" r:id="rId7"/>
-    <hyperlink ref="J31" r:id="rId8"/>
+    <hyperlink ref="J11" r:id="rId1"/>
+    <hyperlink ref="J9" r:id="rId2"/>
+    <hyperlink ref="J10" r:id="rId3"/>
+    <hyperlink ref="J12" r:id="rId4"/>
+    <hyperlink ref="J26" r:id="rId5"/>
+    <hyperlink ref="J30" r:id="rId6"/>
+    <hyperlink ref="J31" r:id="rId7"/>
+    <hyperlink ref="J32" r:id="rId8"/>
     <hyperlink ref="J3" r:id="rId9"/>
     <hyperlink ref="J4" r:id="rId10"/>
     <hyperlink ref="J2" r:id="rId11"/>
     <hyperlink ref="J5" r:id="rId12"/>
     <hyperlink ref="J6" r:id="rId13"/>
     <hyperlink ref="J7" r:id="rId14"/>
-    <hyperlink ref="J12" r:id="rId15"/>
-    <hyperlink ref="J13" r:id="rId16"/>
-    <hyperlink ref="J14" r:id="rId17"/>
-    <hyperlink ref="J15" r:id="rId18"/>
-    <hyperlink ref="J16" r:id="rId19"/>
-    <hyperlink ref="J17" r:id="rId20"/>
-    <hyperlink ref="J18" r:id="rId21"/>
-    <hyperlink ref="J19" r:id="rId22"/>
-    <hyperlink ref="J20" r:id="rId23"/>
-    <hyperlink ref="J21" r:id="rId24"/>
-    <hyperlink ref="J22" r:id="rId25"/>
-    <hyperlink ref="J24" r:id="rId26"/>
-    <hyperlink ref="J23" r:id="rId27"/>
-    <hyperlink ref="J26" r:id="rId28"/>
-    <hyperlink ref="J27" r:id="rId29"/>
-    <hyperlink ref="J28" r:id="rId30"/>
-    <hyperlink ref="J32" r:id="rId31"/>
-    <hyperlink ref="J34" r:id="rId32"/>
-    <hyperlink ref="J35" r:id="rId33"/>
-    <hyperlink ref="J36" r:id="rId34"/>
-    <hyperlink ref="J37" r:id="rId35"/>
-    <hyperlink ref="J38" r:id="rId36"/>
-    <hyperlink ref="J39" r:id="rId37"/>
-    <hyperlink ref="J40" r:id="rId38"/>
-    <hyperlink ref="J41" r:id="rId39"/>
-    <hyperlink ref="J42" r:id="rId40"/>
-    <hyperlink ref="J43" r:id="rId41"/>
-    <hyperlink ref="J44" r:id="rId42"/>
+    <hyperlink ref="J13" r:id="rId15"/>
+    <hyperlink ref="J14" r:id="rId16"/>
+    <hyperlink ref="J15" r:id="rId17"/>
+    <hyperlink ref="J16" r:id="rId18"/>
+    <hyperlink ref="J17" r:id="rId19"/>
+    <hyperlink ref="J18" r:id="rId20"/>
+    <hyperlink ref="J19" r:id="rId21"/>
+    <hyperlink ref="J20" r:id="rId22"/>
+    <hyperlink ref="J21" r:id="rId23"/>
+    <hyperlink ref="J22" r:id="rId24"/>
+    <hyperlink ref="J23" r:id="rId25"/>
+    <hyperlink ref="J25" r:id="rId26"/>
+    <hyperlink ref="J24" r:id="rId27"/>
+    <hyperlink ref="J27" r:id="rId28"/>
+    <hyperlink ref="J28" r:id="rId29"/>
+    <hyperlink ref="J29" r:id="rId30"/>
+    <hyperlink ref="J33" r:id="rId31"/>
+    <hyperlink ref="J35" r:id="rId32"/>
+    <hyperlink ref="J36" r:id="rId33"/>
+    <hyperlink ref="J37" r:id="rId34"/>
+    <hyperlink ref="J38" r:id="rId35"/>
+    <hyperlink ref="J39" r:id="rId36"/>
+    <hyperlink ref="J40" r:id="rId37"/>
+    <hyperlink ref="J41" r:id="rId38"/>
+    <hyperlink ref="J42" r:id="rId39"/>
+    <hyperlink ref="J43" r:id="rId40"/>
+    <hyperlink ref="J44" r:id="rId41"/>
+    <hyperlink ref="J45" r:id="rId42"/>
+    <hyperlink ref="J8" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
full-duplex, 2 ch data, 4 ch alignment working state
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="375">
   <si>
     <t>MFR</t>
   </si>
@@ -1135,6 +1135,24 @@
   </si>
   <si>
     <t>FP-301 1" BL 100'</t>
+  </si>
+  <si>
+    <t>C_POL/20%/RADIAL/25V/16X35</t>
+  </si>
+  <si>
+    <t>MAL225056472E3</t>
+  </si>
+  <si>
+    <t>C5, C6</t>
+  </si>
+  <si>
+    <t>C7, C8</t>
+  </si>
+  <si>
+    <t>RADIAL_21_16_35</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ProductDetail/Vishay-BC-Components/MAL225056472E3/?qs=sGAEpiMZZMsh%252b1woXyUXj60Aw1cMkM73YimYEY6aOaY%3d</t>
   </si>
 </sst>
 </file>
@@ -2657,10 +2675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4061,69 +4079,138 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>357</v>
-      </c>
-      <c r="B46">
-        <v>8</v>
-      </c>
-      <c r="C46" s="45">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D46" s="45">
-        <f>B46*C46</f>
-        <v>8.7200000000000006</v>
-      </c>
-      <c r="E46" t="s">
-        <v>355</v>
-      </c>
-      <c r="F46" t="s">
-        <v>356</v>
-      </c>
-      <c r="G46" t="s">
-        <v>358</v>
-      </c>
-      <c r="H46" t="s">
-        <v>359</v>
-      </c>
-      <c r="J46" s="44" t="s">
-        <v>354</v>
-      </c>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
+        <v>369</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" s="46">
+        <v>4.49</v>
+      </c>
+      <c r="D47" s="45">
+        <f t="shared" ref="D47:D48" si="1">B47*C47</f>
+        <v>8.98</v>
+      </c>
+      <c r="E47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" t="s">
+        <v>370</v>
+      </c>
+      <c r="G47" t="s">
+        <v>371</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="I47" t="s">
+        <v>360</v>
+      </c>
+      <c r="J47" s="44" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>252</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="D48" s="45">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>73</v>
+      </c>
+      <c r="F48" t="s">
+        <v>309</v>
+      </c>
+      <c r="G48" t="s">
+        <v>372</v>
+      </c>
+      <c r="H48" t="s">
+        <v>153</v>
+      </c>
+      <c r="I48" t="s">
+        <v>336</v>
+      </c>
+      <c r="J48" s="44" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>357</v>
+      </c>
+      <c r="B49">
+        <v>8</v>
+      </c>
+      <c r="C49" s="45">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="D49" s="45">
+        <f>B49*C49</f>
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="E49" t="s">
+        <v>355</v>
+      </c>
+      <c r="F49" t="s">
+        <v>356</v>
+      </c>
+      <c r="G49" t="s">
+        <v>358</v>
+      </c>
+      <c r="H49" t="s">
+        <v>359</v>
+      </c>
+      <c r="J49" s="44" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>364</v>
       </c>
-      <c r="B47">
+      <c r="B50">
         <v>1</v>
       </c>
-      <c r="C47" s="45">
+      <c r="C50" s="45">
         <v>5.91</v>
       </c>
-      <c r="D47" s="45">
-        <f>B47*C47</f>
+      <c r="D50" s="45">
+        <f>B50*C50</f>
         <v>5.91</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E50" t="s">
         <v>365</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F50" t="s">
         <v>368</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G50" t="s">
         <v>358</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H50" t="s">
         <v>366</v>
       </c>
-      <c r="J47" s="44" t="s">
+      <c r="J50" s="44" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="D48" s="6">
-        <f>SUM(D2:D47)</f>
-        <v>595.76</v>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="D51" s="6">
+        <f>SUM(D2:D50)</f>
+        <v>604.94000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -4171,9 +4258,11 @@
     <hyperlink ref="J44" r:id="rId41"/>
     <hyperlink ref="J45" r:id="rId42"/>
     <hyperlink ref="J8" r:id="rId43"/>
+    <hyperlink ref="J48" r:id="rId44"/>
+    <hyperlink ref="J47" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 

</xml_diff>